<commit_message>
Working on Crocodile project
</commit_message>
<xml_diff>
--- a/Source/Classic/Apps/Crocodile/Template.xlsx
+++ b/Source/Classic/Apps/Crocodile/Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\ManagedClient.45\Source\Classic\Apps\Crocodile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA17D52-E479-4AFA-8FA1-C948E4FCA7DC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B0B83CB-FF58-4DB1-9354-B5B5C52E51E2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="27630" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -435,7 +435,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add page counting for BookInfo and Crocodile
</commit_message>
<xml_diff>
--- a/Source/Classic/Apps/Crocodile/Template.xlsx
+++ b/Source/Classic/Apps/Crocodile/Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\ManagedClient.45\Source\Classic\Apps\Crocodile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B0B83CB-FF58-4DB1-9354-B5B5C52E51E2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75BCFAC6-33B3-4A29-9BC1-CD482E248F62}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27630" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27720" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>КСУ</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>Фин. эффект.</t>
+  </si>
+  <si>
+    <t>Объем</t>
   </si>
 </sst>
 </file>
@@ -431,11 +434,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,13 +446,14 @@
     <col min="1" max="1" width="79.85546875" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" customWidth="1"/>
     <col min="3" max="3" width="10.28515625" customWidth="1"/>
-    <col min="10" max="10" width="9.42578125" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" customWidth="1"/>
-    <col min="13" max="13" width="13.7109375" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" customWidth="1"/>
+    <col min="13" max="13" width="12.5703125" customWidth="1"/>
+    <col min="14" max="14" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -463,30 +467,33 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>